<commit_message>
Avances del análisis de texto en Español para la short description
</commit_message>
<xml_diff>
--- a/text_analysis/data/long_description_words_goal.xlsx
+++ b/text_analysis/data/long_description_words_goal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5761" uniqueCount="5761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5756" uniqueCount="5756">
   <si>
     <t>children</t>
   </si>
@@ -505,9 +505,6 @@
     <t>basic</t>
   </si>
   <si>
-    <t>para</t>
-  </si>
-  <si>
     <t>create</t>
   </si>
   <si>
@@ -1663,9 +1660,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>país</t>
-  </si>
-  <si>
     <t>clean</t>
   </si>
   <si>
@@ -5557,9 +5551,6 @@
     <t>proposal</t>
   </si>
   <si>
-    <t>visión</t>
-  </si>
-  <si>
     <t>guatemalagivingchallenge</t>
   </si>
   <si>
@@ -7024,9 +7015,6 @@
     <t>galaei</t>
   </si>
   <si>
-    <t>rayón</t>
-  </si>
-  <si>
     <t>collaborations</t>
   </si>
   <si>
@@ -12115,9 +12103,6 @@
     <t>approves</t>
   </si>
   <si>
-    <t>michoacán</t>
-  </si>
-  <si>
     <t>coneval</t>
   </si>
   <si>
@@ -14923,6 +14908,9 @@
     <t>pre-k</t>
   </si>
   <si>
+    <t>goddess</t>
+  </si>
+  <si>
     <t>norm-referenced</t>
   </si>
   <si>
@@ -14951,9 +14939,6 @@
   </si>
   <si>
     <t>productivity</t>
-  </si>
-  <si>
-    <t>goddess</t>
   </si>
   <si>
     <t>nclr</t>
@@ -17654,7 +17639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5762"/>
+  <dimension ref="A1:C5757"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19513,7 +19498,7 @@
         <v>167</v>
       </c>
       <c r="C169">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -19623,7 +19608,7 @@
         <v>177</v>
       </c>
       <c r="C179">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -19799,7 +19784,7 @@
         <v>193</v>
       </c>
       <c r="C195">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -19986,7 +19971,7 @@
         <v>210</v>
       </c>
       <c r="C212">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -20074,7 +20059,7 @@
         <v>218</v>
       </c>
       <c r="C220">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -20206,7 +20191,7 @@
         <v>230</v>
       </c>
       <c r="C232">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -20393,7 +20378,7 @@
         <v>247</v>
       </c>
       <c r="C249">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -20613,7 +20598,7 @@
         <v>267</v>
       </c>
       <c r="C269">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -20943,7 +20928,7 @@
         <v>297</v>
       </c>
       <c r="C299">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="300" spans="1:3">
@@ -21284,7 +21269,7 @@
         <v>328</v>
       </c>
       <c r="C330">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -21702,7 +21687,7 @@
         <v>366</v>
       </c>
       <c r="C368">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="369" spans="1:3">
@@ -22186,7 +22171,7 @@
         <v>410</v>
       </c>
       <c r="C412">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="413" spans="1:3">
@@ -22714,7 +22699,7 @@
         <v>458</v>
       </c>
       <c r="C460">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="461" spans="1:3">
@@ -23385,7 +23370,7 @@
         <v>519</v>
       </c>
       <c r="C521">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="522" spans="1:3">
@@ -24276,7 +24261,7 @@
         <v>600</v>
       </c>
       <c r="C602">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="603" spans="1:3">
@@ -24287,7 +24272,7 @@
         <v>601</v>
       </c>
       <c r="C603">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="604" spans="1:3">
@@ -25442,7 +25427,7 @@
         <v>706</v>
       </c>
       <c r="C708">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="709" spans="1:3">
@@ -25453,7 +25438,7 @@
         <v>707</v>
       </c>
       <c r="C709">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="710" spans="1:3">
@@ -26674,7 +26659,7 @@
         <v>818</v>
       </c>
       <c r="C820">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="821" spans="1:3">
@@ -26685,7 +26670,7 @@
         <v>819</v>
       </c>
       <c r="C821">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="822" spans="1:3">
@@ -28269,7 +28254,7 @@
         <v>963</v>
       </c>
       <c r="C965">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="966" spans="1:3">
@@ -28280,7 +28265,7 @@
         <v>964</v>
       </c>
       <c r="C966">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="967" spans="1:3">
@@ -30645,7 +30630,7 @@
         <v>1179</v>
       </c>
       <c r="C1181">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1182" spans="1:3">
@@ -30656,7 +30641,7 @@
         <v>1180</v>
       </c>
       <c r="C1182">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1183" spans="1:3">
@@ -33956,7 +33941,7 @@
         <v>1480</v>
       </c>
       <c r="C1482">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1483" spans="1:3">
@@ -33967,7 +33952,7 @@
         <v>1481</v>
       </c>
       <c r="C1483">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1484" spans="1:3">
@@ -39192,7 +39177,7 @@
         <v>1956</v>
       </c>
       <c r="C1958">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1959" spans="1:3">
@@ -39203,7 +39188,7 @@
         <v>1957</v>
       </c>
       <c r="C1959">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1960" spans="1:3">
@@ -39214,7 +39199,7 @@
         <v>1958</v>
       </c>
       <c r="C1960">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1961" spans="1:3">
@@ -49708,7 +49693,7 @@
         <v>2912</v>
       </c>
       <c r="C2914">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2915" spans="1:3">
@@ -49719,7 +49704,7 @@
         <v>2913</v>
       </c>
       <c r="C2915">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2916" spans="1:3">
@@ -49730,7 +49715,7 @@
         <v>2914</v>
       </c>
       <c r="C2916">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2917" spans="1:3">
@@ -49741,7 +49726,7 @@
         <v>2915</v>
       </c>
       <c r="C2917">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2918" spans="1:3">
@@ -80981,61 +80966,6 @@
         <v>5755</v>
       </c>
       <c r="C5757">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5758" spans="1:3">
-      <c r="A5758" s="1">
-        <v>5756</v>
-      </c>
-      <c r="B5758" t="s">
-        <v>5756</v>
-      </c>
-      <c r="C5758">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5759" spans="1:3">
-      <c r="A5759" s="1">
-        <v>5757</v>
-      </c>
-      <c r="B5759" t="s">
-        <v>5757</v>
-      </c>
-      <c r="C5759">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5760" spans="1:3">
-      <c r="A5760" s="1">
-        <v>5758</v>
-      </c>
-      <c r="B5760" t="s">
-        <v>5758</v>
-      </c>
-      <c r="C5760">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5761" spans="1:3">
-      <c r="A5761" s="1">
-        <v>5759</v>
-      </c>
-      <c r="B5761" t="s">
-        <v>5759</v>
-      </c>
-      <c r="C5761">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5762" spans="1:3">
-      <c r="A5762" s="1">
-        <v>5760</v>
-      </c>
-      <c r="B5762" t="s">
-        <v>5760</v>
-      </c>
-      <c r="C5762">
         <v>1</v>
       </c>
     </row>

</xml_diff>